<commit_message>
Mejorando graficas de malla
</commit_message>
<xml_diff>
--- a/metrics/MAPE/Amputación extremidades inferiores.xlsx
+++ b/metrics/MAPE/Amputación extremidades inferiores.xlsx
@@ -478,13 +478,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.02135272098885925</v>
+        <v>0.0211044387209215</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0214137136774855</v>
+        <v>0.0215360816073263</v>
       </c>
       <c r="D3" t="n">
-        <v>0.02134150529475662</v>
+        <v>0.02139758049042934</v>
       </c>
     </row>
     <row r="4">
@@ -510,13 +510,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.03286466251641493</v>
+        <v>0.03350579708030758</v>
       </c>
       <c r="C5" t="n">
-        <v>0.03208925550964176</v>
+        <v>0.03379712648029576</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0326837156506363</v>
+        <v>0.0340434936785425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>